<commit_message>
RDM-4687 - add conditional show hide tests for collection of complex fields
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v06_collection_view.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v06_collection_view.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\moj\ccd-case-management-web\test\resources\definitionsFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32EAA6C-00A4-4C3B-ACC4-C6E63CBF16FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85184C64-7C82-4B69-AA5F-3FD6414F6813}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="507" windowWidth="25786" windowHeight="13986" tabRatio="683" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="507" windowWidth="25786" windowHeight="13986" tabRatio="807" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2076" uniqueCount="511">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1642,6 +1642,18 @@
   </si>
   <si>
     <t>TextField3="showpage3"</t>
+  </si>
+  <si>
+    <t>Collection of Addresses</t>
+  </si>
+  <si>
+    <t>ConditionalPage4</t>
+  </si>
+  <si>
+    <t>Conditional Page 4</t>
+  </si>
+  <si>
+    <t>TextField3="showpage4"</t>
   </si>
 </sst>
 </file>
@@ -3634,10 +3646,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AD46"/>
+  <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -6022,6 +6034,59 @@
       <c r="AA46" s="157"/>
       <c r="AB46" s="157"/>
       <c r="AC46" s="157"/>
+    </row>
+    <row r="47" spans="1:29" s="154" customFormat="1" ht="13.75" customHeight="1">
+      <c r="A47" s="155">
+        <v>42736</v>
+      </c>
+      <c r="B47" s="155"/>
+      <c r="C47" s="156" t="s">
+        <v>398</v>
+      </c>
+      <c r="D47" s="156" t="s">
+        <v>193</v>
+      </c>
+      <c r="E47" s="158" t="s">
+        <v>479</v>
+      </c>
+      <c r="F47" s="159">
+        <v>1</v>
+      </c>
+      <c r="G47" s="156" t="s">
+        <v>346</v>
+      </c>
+      <c r="H47" s="158" t="s">
+        <v>508</v>
+      </c>
+      <c r="I47" s="158" t="s">
+        <v>509</v>
+      </c>
+      <c r="J47" s="160">
+        <v>4</v>
+      </c>
+      <c r="K47" s="157"/>
+      <c r="L47" s="153"/>
+      <c r="M47" s="161" t="s">
+        <v>510</v>
+      </c>
+      <c r="N47" s="157"/>
+      <c r="O47" s="156" t="s">
+        <v>195</v>
+      </c>
+      <c r="P47" s="157"/>
+      <c r="Q47" s="157"/>
+      <c r="R47" s="157"/>
+      <c r="S47" s="157"/>
+      <c r="T47" s="157"/>
+      <c r="U47" s="157"/>
+      <c r="V47" s="157"/>
+      <c r="W47" s="157"/>
+      <c r="X47" s="157"/>
+      <c r="Y47" s="157"/>
+      <c r="Z47" s="157"/>
+      <c r="AA47" s="157"/>
+      <c r="AB47" s="157"/>
+      <c r="AC47" s="157"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -7656,10 +7721,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -8860,6 +8925,29 @@
       <c r="I52" s="157"/>
       <c r="J52" s="157"/>
       <c r="K52" s="157"/>
+    </row>
+    <row r="53" spans="1:11" s="154" customFormat="1" ht="13.75" customHeight="1">
+      <c r="A53" s="155">
+        <v>42736</v>
+      </c>
+      <c r="B53" s="155"/>
+      <c r="C53" s="156" t="s">
+        <v>398</v>
+      </c>
+      <c r="D53" s="158" t="s">
+        <v>479</v>
+      </c>
+      <c r="E53" s="154" t="s">
+        <v>271</v>
+      </c>
+      <c r="F53" s="156" t="s">
+        <v>244</v>
+      </c>
+      <c r="G53" s="156"/>
+      <c r="H53" s="157"/>
+      <c r="I53" s="157"/>
+      <c r="J53" s="157"/>
+      <c r="K53" s="157"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -10132,10 +10220,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV53"/>
+  <dimension ref="A1:IV54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -20647,6 +20735,278 @@
       <c r="IU53" s="153"/>
       <c r="IV53" s="153"/>
     </row>
+    <row r="54" spans="1:256" s="154" customFormat="1" ht="13.75" customHeight="1">
+      <c r="A54" s="148">
+        <v>42736</v>
+      </c>
+      <c r="B54" s="149"/>
+      <c r="C54" s="150" t="s">
+        <v>398</v>
+      </c>
+      <c r="D54" s="151" t="s">
+        <v>479</v>
+      </c>
+      <c r="E54" s="151" t="s">
+        <v>507</v>
+      </c>
+      <c r="F54" s="152"/>
+      <c r="G54" s="151" t="s">
+        <v>64</v>
+      </c>
+      <c r="H54" s="152" t="s">
+        <v>51</v>
+      </c>
+      <c r="I54" s="152"/>
+      <c r="J54" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="K54" s="152"/>
+      <c r="L54" s="152"/>
+      <c r="M54" s="152"/>
+      <c r="N54" s="152"/>
+      <c r="O54" s="152"/>
+      <c r="P54" s="152"/>
+      <c r="Q54" s="152"/>
+      <c r="R54" s="153"/>
+      <c r="S54" s="153"/>
+      <c r="T54" s="153"/>
+      <c r="U54" s="153"/>
+      <c r="V54" s="153"/>
+      <c r="W54" s="153"/>
+      <c r="X54" s="153"/>
+      <c r="Y54" s="153"/>
+      <c r="Z54" s="153"/>
+      <c r="AA54" s="153"/>
+      <c r="AB54" s="153"/>
+      <c r="AC54" s="153"/>
+      <c r="AD54" s="153"/>
+      <c r="AE54" s="153"/>
+      <c r="AF54" s="153"/>
+      <c r="AG54" s="153"/>
+      <c r="AH54" s="153"/>
+      <c r="AI54" s="153"/>
+      <c r="AJ54" s="153"/>
+      <c r="AK54" s="153"/>
+      <c r="AL54" s="153"/>
+      <c r="AM54" s="153"/>
+      <c r="AN54" s="153"/>
+      <c r="AO54" s="153"/>
+      <c r="AP54" s="153"/>
+      <c r="AQ54" s="153"/>
+      <c r="AR54" s="153"/>
+      <c r="AS54" s="153"/>
+      <c r="AT54" s="153"/>
+      <c r="AU54" s="153"/>
+      <c r="AV54" s="153"/>
+      <c r="AW54" s="153"/>
+      <c r="AX54" s="153"/>
+      <c r="AY54" s="153"/>
+      <c r="AZ54" s="153"/>
+      <c r="BA54" s="153"/>
+      <c r="BB54" s="153"/>
+      <c r="BC54" s="153"/>
+      <c r="BD54" s="153"/>
+      <c r="BE54" s="153"/>
+      <c r="BF54" s="153"/>
+      <c r="BG54" s="153"/>
+      <c r="BH54" s="153"/>
+      <c r="BI54" s="153"/>
+      <c r="BJ54" s="153"/>
+      <c r="BK54" s="153"/>
+      <c r="BL54" s="153"/>
+      <c r="BM54" s="153"/>
+      <c r="BN54" s="153"/>
+      <c r="BO54" s="153"/>
+      <c r="BP54" s="153"/>
+      <c r="BQ54" s="153"/>
+      <c r="BR54" s="153"/>
+      <c r="BS54" s="153"/>
+      <c r="BT54" s="153"/>
+      <c r="BU54" s="153"/>
+      <c r="BV54" s="153"/>
+      <c r="BW54" s="153"/>
+      <c r="BX54" s="153"/>
+      <c r="BY54" s="153"/>
+      <c r="BZ54" s="153"/>
+      <c r="CA54" s="153"/>
+      <c r="CB54" s="153"/>
+      <c r="CC54" s="153"/>
+      <c r="CD54" s="153"/>
+      <c r="CE54" s="153"/>
+      <c r="CF54" s="153"/>
+      <c r="CG54" s="153"/>
+      <c r="CH54" s="153"/>
+      <c r="CI54" s="153"/>
+      <c r="CJ54" s="153"/>
+      <c r="CK54" s="153"/>
+      <c r="CL54" s="153"/>
+      <c r="CM54" s="153"/>
+      <c r="CN54" s="153"/>
+      <c r="CO54" s="153"/>
+      <c r="CP54" s="153"/>
+      <c r="CQ54" s="153"/>
+      <c r="CR54" s="153"/>
+      <c r="CS54" s="153"/>
+      <c r="CT54" s="153"/>
+      <c r="CU54" s="153"/>
+      <c r="CV54" s="153"/>
+      <c r="CW54" s="153"/>
+      <c r="CX54" s="153"/>
+      <c r="CY54" s="153"/>
+      <c r="CZ54" s="153"/>
+      <c r="DA54" s="153"/>
+      <c r="DB54" s="153"/>
+      <c r="DC54" s="153"/>
+      <c r="DD54" s="153"/>
+      <c r="DE54" s="153"/>
+      <c r="DF54" s="153"/>
+      <c r="DG54" s="153"/>
+      <c r="DH54" s="153"/>
+      <c r="DI54" s="153"/>
+      <c r="DJ54" s="153"/>
+      <c r="DK54" s="153"/>
+      <c r="DL54" s="153"/>
+      <c r="DM54" s="153"/>
+      <c r="DN54" s="153"/>
+      <c r="DO54" s="153"/>
+      <c r="DP54" s="153"/>
+      <c r="DQ54" s="153"/>
+      <c r="DR54" s="153"/>
+      <c r="DS54" s="153"/>
+      <c r="DT54" s="153"/>
+      <c r="DU54" s="153"/>
+      <c r="DV54" s="153"/>
+      <c r="DW54" s="153"/>
+      <c r="DX54" s="153"/>
+      <c r="DY54" s="153"/>
+      <c r="DZ54" s="153"/>
+      <c r="EA54" s="153"/>
+      <c r="EB54" s="153"/>
+      <c r="EC54" s="153"/>
+      <c r="ED54" s="153"/>
+      <c r="EE54" s="153"/>
+      <c r="EF54" s="153"/>
+      <c r="EG54" s="153"/>
+      <c r="EH54" s="153"/>
+      <c r="EI54" s="153"/>
+      <c r="EJ54" s="153"/>
+      <c r="EK54" s="153"/>
+      <c r="EL54" s="153"/>
+      <c r="EM54" s="153"/>
+      <c r="EN54" s="153"/>
+      <c r="EO54" s="153"/>
+      <c r="EP54" s="153"/>
+      <c r="EQ54" s="153"/>
+      <c r="ER54" s="153"/>
+      <c r="ES54" s="153"/>
+      <c r="ET54" s="153"/>
+      <c r="EU54" s="153"/>
+      <c r="EV54" s="153"/>
+      <c r="EW54" s="153"/>
+      <c r="EX54" s="153"/>
+      <c r="EY54" s="153"/>
+      <c r="EZ54" s="153"/>
+      <c r="FA54" s="153"/>
+      <c r="FB54" s="153"/>
+      <c r="FC54" s="153"/>
+      <c r="FD54" s="153"/>
+      <c r="FE54" s="153"/>
+      <c r="FF54" s="153"/>
+      <c r="FG54" s="153"/>
+      <c r="FH54" s="153"/>
+      <c r="FI54" s="153"/>
+      <c r="FJ54" s="153"/>
+      <c r="FK54" s="153"/>
+      <c r="FL54" s="153"/>
+      <c r="FM54" s="153"/>
+      <c r="FN54" s="153"/>
+      <c r="FO54" s="153"/>
+      <c r="FP54" s="153"/>
+      <c r="FQ54" s="153"/>
+      <c r="FR54" s="153"/>
+      <c r="FS54" s="153"/>
+      <c r="FT54" s="153"/>
+      <c r="FU54" s="153"/>
+      <c r="FV54" s="153"/>
+      <c r="FW54" s="153"/>
+      <c r="FX54" s="153"/>
+      <c r="FY54" s="153"/>
+      <c r="FZ54" s="153"/>
+      <c r="GA54" s="153"/>
+      <c r="GB54" s="153"/>
+      <c r="GC54" s="153"/>
+      <c r="GD54" s="153"/>
+      <c r="GE54" s="153"/>
+      <c r="GF54" s="153"/>
+      <c r="GG54" s="153"/>
+      <c r="GH54" s="153"/>
+      <c r="GI54" s="153"/>
+      <c r="GJ54" s="153"/>
+      <c r="GK54" s="153"/>
+      <c r="GL54" s="153"/>
+      <c r="GM54" s="153"/>
+      <c r="GN54" s="153"/>
+      <c r="GO54" s="153"/>
+      <c r="GP54" s="153"/>
+      <c r="GQ54" s="153"/>
+      <c r="GR54" s="153"/>
+      <c r="GS54" s="153"/>
+      <c r="GT54" s="153"/>
+      <c r="GU54" s="153"/>
+      <c r="GV54" s="153"/>
+      <c r="GW54" s="153"/>
+      <c r="GX54" s="153"/>
+      <c r="GY54" s="153"/>
+      <c r="GZ54" s="153"/>
+      <c r="HA54" s="153"/>
+      <c r="HB54" s="153"/>
+      <c r="HC54" s="153"/>
+      <c r="HD54" s="153"/>
+      <c r="HE54" s="153"/>
+      <c r="HF54" s="153"/>
+      <c r="HG54" s="153"/>
+      <c r="HH54" s="153"/>
+      <c r="HI54" s="153"/>
+      <c r="HJ54" s="153"/>
+      <c r="HK54" s="153"/>
+      <c r="HL54" s="153"/>
+      <c r="HM54" s="153"/>
+      <c r="HN54" s="153"/>
+      <c r="HO54" s="153"/>
+      <c r="HP54" s="153"/>
+      <c r="HQ54" s="153"/>
+      <c r="HR54" s="153"/>
+      <c r="HS54" s="153"/>
+      <c r="HT54" s="153"/>
+      <c r="HU54" s="153"/>
+      <c r="HV54" s="153"/>
+      <c r="HW54" s="153"/>
+      <c r="HX54" s="153"/>
+      <c r="HY54" s="153"/>
+      <c r="HZ54" s="153"/>
+      <c r="IA54" s="153"/>
+      <c r="IB54" s="153"/>
+      <c r="IC54" s="153"/>
+      <c r="ID54" s="153"/>
+      <c r="IE54" s="153"/>
+      <c r="IF54" s="153"/>
+      <c r="IG54" s="153"/>
+      <c r="IH54" s="153"/>
+      <c r="II54" s="153"/>
+      <c r="IJ54" s="153"/>
+      <c r="IK54" s="153"/>
+      <c r="IL54" s="153"/>
+      <c r="IM54" s="153"/>
+      <c r="IN54" s="153"/>
+      <c r="IO54" s="153"/>
+      <c r="IP54" s="153"/>
+      <c r="IQ54" s="153"/>
+      <c r="IR54" s="153"/>
+      <c r="IS54" s="153"/>
+      <c r="IT54" s="153"/>
+      <c r="IU54" s="153"/>
+      <c r="IV54" s="153"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -20660,7 +21020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>